<commit_message>
I made some levels
Yeah
</commit_message>
<xml_diff>
--- a/Demo/DemoResults/PuzzleTimes.xlsx
+++ b/Demo/DemoResults/PuzzleTimes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevo\Documents\DokiDokiConga\Demo\DemoResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABAF636-3E69-4D2D-B68C-6314E80CBEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3256A756-6372-4A5E-9B0F-637F3B07935A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6630" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>Puzzle #</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>Bad</t>
+  </si>
+  <si>
+    <t>Sci-fi</t>
+  </si>
+  <si>
+    <t>Party?</t>
   </si>
 </sst>
 </file>
@@ -214,7 +220,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +245,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -255,13 +267,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60% - Accent2" xfId="1" builtinId="36"/>
@@ -548,7 +561,7 @@
   <dimension ref="A1:AC31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,17 +590,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F1" t="s">
         <v>46</v>
       </c>
       <c r="H1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="J1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="L1" t="s">
         <v>46</v>
@@ -595,7 +608,7 @@
       <c r="N1" t="s">
         <v>48</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="4" t="s">
         <v>47</v>
       </c>
       <c r="R1" t="s">
@@ -607,7 +620,7 @@
       <c r="X1" t="s">
         <v>50</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="4" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>